<commit_message>
pr 5 terminada (menos punto 24)
</commit_message>
<xml_diff>
--- a/PRACTICAS/PRACTICA_5/Punto22.xlsx
+++ b/PRACTICAS/PRACTICA_5/Punto22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Agus\Escritorio\Facultad\2DO AÑO\2do_Semestre\ISO\PRACTICAS\PRACTICA_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86C1776-5711-472D-9591-0D9EAF8BEDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAAF4FE-B16B-424D-83D6-1A17DBFCDC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C6C00091-BCC9-4793-8423-6921387DE014}"/>
   </bookViews>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E92B35B-004C-4C92-B1C8-E47A62FB5E40}">
   <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="AF56" sqref="AF56"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="AE24" sqref="AE24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>